<commit_message>
feat: adding new scrippts for scraping
</commit_message>
<xml_diff>
--- a/extract_details/outputs/mundoverde-vitaminas.xlsx
+++ b/extract_details/outputs/mundoverde-vitaminas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KRUSS\Documents\web_scraping\proyecto_bra\finals\web-scraping-thomas\outputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KRUSS\Documents\web_scraping\proyecto_bra\finals\web-scraping-thomas\extract_details\outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -762,10 +762,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1072,16 +1075,18 @@
   <dimension ref="A1:F58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" customWidth="1"/>
-    <col min="2" max="2" width="46.42578125" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" customWidth="1"/>
-    <col min="4" max="4" width="37.28515625" customWidth="1"/>
-    <col min="6" max="6" width="89" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="59.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="37.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="24" style="2" customWidth="1"/>
+    <col min="6" max="6" width="97" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1105,992 +1110,992 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="2" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="2" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="2" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="2" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="2" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="2" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="2" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="2" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="2" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="2" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="2" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="2" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="2" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="2" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="2" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="2" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="2" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="A27" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" s="2" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="A28" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F28" s="2" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="A29" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29" s="2" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="A30" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F30" s="2" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="A31" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F31" s="2" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="A32" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F32" s="2" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="A33" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F33" s="2" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="A34" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F34" s="2" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="A35" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F35" s="2" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="A36" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E36" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F36" s="2" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="A37" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F37" s="2" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="A38" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F38" s="2" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="A39" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E39" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F39" s="2" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="A40" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F40" s="2" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="A41" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E41" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F41" s="2" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="A42" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E42" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F42" s="2" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="A43" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E43" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F43" t="s">
+      <c r="F43" s="2" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="A44" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E44" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F44" s="2" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="A45" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E45" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F45" t="s">
+      <c r="F45" s="2" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="A46" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E46" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F46" t="s">
+      <c r="F46" s="2" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="A47" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E47" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F47" t="s">
+      <c r="F47" s="2" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="A48" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E48" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F48" t="s">
+      <c r="F48" s="2" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="A49" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E49" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F49" t="s">
+      <c r="F49" s="2" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="A50" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E50" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F50" t="s">
+      <c r="F50" s="2" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="A51" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E51" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F51" t="s">
+      <c r="F51" s="2" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="A52" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E52" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F52" t="s">
+      <c r="F52" s="2" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+      <c r="A53" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E53" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F53" t="s">
+      <c r="F53" s="2" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+      <c r="A54" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E54" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F54" t="s">
+      <c r="F54" s="2" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="A55" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E55" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F55" t="s">
+      <c r="F55" s="2" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+      <c r="A56" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E56" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F56" t="s">
+      <c r="F56" s="2" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+      <c r="A57" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="E57" t="s">
+      <c r="E57" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F57" t="s">
+      <c r="F57" s="2" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+      <c r="A58" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="E58" t="s">
+      <c r="E58" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F58" t="s">
+      <c r="F58" s="2" t="s">
         <v>228</v>
       </c>
     </row>

</xml_diff>